<commit_message>
FIX issue #177: Change `.status` to `.cancelled`, and add `.active` where missing
</commit_message>
<xml_diff>
--- a/tools/logistics.xlsx
+++ b/tools/logistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UW31RY\work\papiNet-API\3.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UW31RY\work\papiNet-API\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB70830B-66FE-4CB9-B5AB-FD2507CA59DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18F3C7A-3D7B-4BDA-A260-6F1AD8DBC3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9275D04F-88B9-4E47-99DB-5102E40C57F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="73">
   <si>
     <t>ListOfSupplierOrders</t>
   </si>
@@ -59,9 +59,6 @@
     <t>number</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>active</t>
   </si>
   <si>
@@ -252,13 +249,32 @@
   </si>
   <si>
     <t>logisticsDeliveryParty</t>
+  </si>
+  <si>
+    <r>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mistake)</t>
+    </r>
+  </si>
+  <si>
+    <t>cancelled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +325,31 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -410,9 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -513,6 +551,24 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -945,9 +1001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678FAC13-5025-4250-BD51-DD8155D9A76B}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,45 +1028,45 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
-        <v>49</v>
+      <c r="A3" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="41" t="s">
-        <v>49</v>
+      <c r="C3" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="41" t="s">
-        <v>49</v>
+      <c r="F3" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="G3" s="11"/>
     </row>
@@ -1084,53 +1140,59 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>7</v>
+      <c r="A7" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>7</v>
+      </c>
       <c r="F8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1142,28 +1204,28 @@
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="7"/>
@@ -1173,33 +1235,33 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>9</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>70</v>
+      <c r="A14" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>69</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1207,10 +1269,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="7"/>
@@ -1220,12 +1282,12 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="15"/>
+        <v>11</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -1235,10 +1297,10 @@
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1248,10 +1310,10 @@
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1263,7 +1325,7 @@
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
       <c r="E19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1274,7 +1336,7 @@
       <c r="C20" s="8"/>
       <c r="D20" s="7"/>
       <c r="E20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -1284,8 +1346,8 @@
       <c r="B21" s="9"/>
       <c r="C21" s="8"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="2" t="s">
-        <v>62</v>
+      <c r="E21" s="56" t="s">
+        <v>61</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1296,125 +1358,125 @@
       <c r="C22" s="8"/>
       <c r="D22" s="7"/>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="11"/>
       <c r="E23" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="44"/>
+      <c r="E25" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="30"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="31" t="s">
         <v>68</v>
       </c>
+      <c r="G26" s="30" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="22"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="3" t="s">
-        <v>7</v>
+      <c r="A28" s="24"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="54" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="35" t="s">
-        <v>10</v>
+      <c r="A29" s="24"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="34" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="48" t="s">
-        <v>71</v>
+      <c r="A30" s="24"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="47" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="37" t="s">
-        <v>12</v>
+      <c r="A31" s="24"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="36" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="39" t="s">
-        <v>50</v>
+      <c r="D32" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="38" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1435,12 +1497,12 @@
       <c r="B34" s="9"/>
       <c r="C34" s="8"/>
       <c r="D34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1448,12 +1510,12 @@
       <c r="B35" s="9"/>
       <c r="C35" s="8"/>
       <c r="D35" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1461,12 +1523,12 @@
       <c r="B36" s="9"/>
       <c r="C36" s="8"/>
       <c r="D36" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1474,12 +1536,12 @@
       <c r="B37" s="9"/>
       <c r="C37" s="8"/>
       <c r="D37" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1487,12 +1549,12 @@
       <c r="B38" s="9"/>
       <c r="C38" s="8"/>
       <c r="D38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1500,12 +1562,12 @@
       <c r="B39" s="9"/>
       <c r="C39" s="8"/>
       <c r="D39" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1513,12 +1575,12 @@
       <c r="B40" s="9"/>
       <c r="C40" s="8"/>
       <c r="D40" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1526,12 +1588,12 @@
       <c r="B41" s="9"/>
       <c r="C41" s="8"/>
       <c r="D41" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1539,12 +1601,12 @@
       <c r="B42" s="9"/>
       <c r="C42" s="8"/>
       <c r="D42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1552,12 +1614,12 @@
       <c r="B43" s="9"/>
       <c r="C43" s="8"/>
       <c r="D43" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1565,12 +1627,12 @@
       <c r="B44" s="9"/>
       <c r="C44" s="8"/>
       <c r="D44" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1578,12 +1640,12 @@
       <c r="B45" s="9"/>
       <c r="C45" s="8"/>
       <c r="D45" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1591,12 +1653,12 @@
       <c r="B46" s="9"/>
       <c r="C46" s="8"/>
       <c r="D46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1604,12 +1666,12 @@
       <c r="B47" s="9"/>
       <c r="C47" s="8"/>
       <c r="D47" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1617,12 +1679,12 @@
       <c r="B48" s="9"/>
       <c r="C48" s="8"/>
       <c r="D48" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1630,46 +1692,46 @@
       <c r="B49" s="9"/>
       <c r="C49" s="8"/>
       <c r="D49" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="17" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="14"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="18" t="s">
-        <v>36</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
-      <c r="G50" s="24" t="s">
-        <v>36</v>
+      <c r="G50" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="31" t="s">
-        <v>52</v>
+        <v>12</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>52</v>
+        <v>12</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="F51" s="7"/>
-      <c r="G51" s="32" t="s">
-        <v>52</v>
+      <c r="G51" s="31" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1685,189 +1747,189 @@
         <v>6</v>
       </c>
       <c r="F52" s="7"/>
-      <c r="G52" s="33" t="s">
+      <c r="G52" s="32" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="22"/>
-      <c r="B53" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="22"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="21"/>
+      <c r="D53" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" s="21"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="28" t="s">
-        <v>58</v>
+      <c r="A54" s="25"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="22"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="19" t="s">
+      <c r="A55" s="21"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="E56" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="19" t="s">
+      <c r="F56" s="7"/>
+      <c r="G56" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="22"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="19" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="21"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E57" s="21"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="22"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="19" t="s">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="21"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E57" s="22"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="19" t="s">
+      <c r="E58" s="21"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="22"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="19" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="21"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E58" s="22"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="22"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E59" s="22"/>
+      <c r="E59" s="21"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="22"/>
-      <c r="B60" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="22"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="21"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="22"/>
-      <c r="B61" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="22"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="21"/>
+      <c r="D61" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="21"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="22"/>
-      <c r="B62" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="22"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="21"/>
+      <c r="D62" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="21"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="19" t="s">
-        <v>17</v>
+      <c r="G62" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="11"/>
-      <c r="B63" s="14"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="11"/>
-      <c r="D63" s="14"/>
+      <c r="D63" s="13"/>
       <c r="E63" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="23"/>
-      <c r="B64" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64" s="23"/>
-      <c r="D64" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="20" t="s">
-        <v>18</v>
+      <c r="A64" s="22"/>
+      <c r="B64" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="22"/>
+      <c r="D64" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="F64" s="7"/>
-      <c r="G64" s="20" t="s">
-        <v>18</v>
+      <c r="G64" s="19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="11"/>
       <c r="B65" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
       <c r="G65" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="7"/>
       <c r="B66" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -1880,12 +1942,12 @@
       <c r="B67" s="8"/>
       <c r="C67" s="7"/>
       <c r="D67" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -1893,31 +1955,31 @@
       <c r="B68" s="8"/>
       <c r="C68" s="7"/>
       <c r="D68" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="11"/>
-      <c r="B69" s="14"/>
+      <c r="B69" s="13"/>
       <c r="C69" s="11"/>
       <c r="D69" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="7"/>
-      <c r="B70" s="32" t="s">
-        <v>50</v>
+      <c r="B70" s="31" t="s">
+        <v>49</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -1939,7 +2001,7 @@
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="7"/>
       <c r="B72" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -1950,7 +2012,7 @@
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="7"/>
       <c r="B73" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -1961,7 +2023,7 @@
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="7"/>
       <c r="B74" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -1972,7 +2034,7 @@
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="7"/>
       <c r="B75" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -1983,7 +2045,7 @@
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="7"/>
       <c r="B76" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -1994,7 +2056,7 @@
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="7"/>
       <c r="B77" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -2005,7 +2067,7 @@
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="7"/>
       <c r="B78" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -2016,7 +2078,7 @@
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="7"/>
       <c r="B79" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -2027,7 +2089,7 @@
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="7"/>
       <c r="B80" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -2038,7 +2100,7 @@
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="7"/>
       <c r="B81" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -2049,7 +2111,7 @@
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="7"/>
       <c r="B82" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -2060,7 +2122,7 @@
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="7"/>
       <c r="B83" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -2071,7 +2133,7 @@
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="7"/>
       <c r="B84" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -2082,7 +2144,7 @@
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="7"/>
       <c r="B85" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -2093,7 +2155,7 @@
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="7"/>
       <c r="B86" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -2104,7 +2166,7 @@
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="7"/>
       <c r="B87" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -2114,8 +2176,8 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="11"/>
-      <c r="B88" s="24" t="s">
-        <v>36</v>
+      <c r="B88" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -2126,18 +2188,18 @@
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="11"/>
       <c r="B89" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F89" s="16"/>
+        <v>52</v>
+      </c>
+      <c r="F89" s="15"/>
       <c r="G89" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -2145,14 +2207,14 @@
       <c r="B90" s="8"/>
       <c r="C90" s="7"/>
       <c r="D90" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -2160,14 +2222,14 @@
       <c r="B91" s="8"/>
       <c r="C91" s="7"/>
       <c r="D91" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -2175,14 +2237,14 @@
       <c r="B92" s="8"/>
       <c r="C92" s="7"/>
       <c r="D92" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -2190,45 +2252,45 @@
       <c r="B93" s="8"/>
       <c r="C93" s="7"/>
       <c r="D93" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="11"/>
-      <c r="B94" s="14"/>
+      <c r="B94" s="13"/>
       <c r="C94" s="11"/>
-      <c r="D94" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E94" s="21" t="s">
-        <v>53</v>
+      <c r="D94" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="F94" s="11"/>
-      <c r="G94" s="21" t="s">
-        <v>53</v>
+      <c r="G94" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B95" s="16"/>
-      <c r="C95" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D95" s="16"/>
-      <c r="E95" s="16"/>
-      <c r="F95" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="16"/>
+      <c r="A95" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" s="15"/>
+      <c r="C95" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>